<commit_message>
Se avanza con las graficas generadas
</commit_message>
<xml_diff>
--- a/Experimento2/Laboratorio de Electronica Analógica.xlsx
+++ b/Experimento2/Laboratorio de Electronica Analógica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d4v1d\Desktop\LabAnalogicaGraficas\GIT\Laboratorio_Electronica_Analogica\Experimento2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71723399-EF3C-4153-A8AE-0AEFF9236A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E4724-3FEA-4AA1-A37B-ADBDAECA4C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="9180" windowWidth="21600" windowHeight="6000" activeTab="1" xr2:uid="{780E1F5D-033D-4143-B95C-BD9CFB1DEE27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{780E1F5D-033D-4143-B95C-BD9CFB1DEE27}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimento 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="92">
   <si>
     <t>vf</t>
   </si>
@@ -7527,8 +7527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52119BB-0D04-7345-A8DD-30782BE70CA4}">
   <dimension ref="A6:Y72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7657,6 +7657,9 @@
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
@@ -7665,6 +7668,9 @@
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -7680,7 +7686,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="L17" s="8" t="s">
         <v>15</v>
       </c>
@@ -7692,7 +7698,7 @@
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>85</v>
       </c>
@@ -7727,7 +7733,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>34</v>
       </c>
@@ -7756,7 +7762,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="L20" s="6">
         <v>7.0720000000000001</v>
       </c>
@@ -7772,7 +7778,7 @@
       </c>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>35</v>
       </c>
@@ -7786,7 +7792,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>36</v>
       </c>
@@ -7800,7 +7806,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="O23">
         <v>7.54</v>
       </c>
@@ -7808,7 +7814,10 @@
         <v>0.13669999999999999</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
       <c r="B25" t="s">
         <v>38</v>
       </c>
@@ -7816,12 +7825,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>91</v>
+      </c>
       <c r="C26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
       <c r="C27" t="s">
         <v>41</v>
       </c>
@@ -7829,7 +7844,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
       <c r="C28" t="s">
         <v>42</v>
       </c>
@@ -7837,7 +7855,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>44</v>
       </c>
@@ -7851,7 +7869,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>80</v>
       </c>
@@ -8030,7 +8048,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>89</v>
       </c>
@@ -8044,7 +8062,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>90</v>
       </c>
@@ -8052,7 +8070,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>91</v>
       </c>
@@ -8069,7 +8087,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>92</v>
       </c>
@@ -8077,12 +8095,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q53">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q54">
         <v>110</v>
       </c>
@@ -8090,7 +8108,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>57</v>
       </c>
@@ -8104,7 +8122,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>59</v>
       </c>
@@ -8112,7 +8130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>64</v>
       </c>
@@ -8126,7 +8144,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>63</v>
       </c>
@@ -8134,7 +8152,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>91</v>
+      </c>
       <c r="C60" t="s">
         <v>65</v>
       </c>
@@ -8142,12 +8163,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>91</v>
+      </c>
       <c r="C61" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
       <c r="C62" t="s">
         <v>67</v>
       </c>
@@ -8155,12 +8182,18 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="63" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
       <c r="C63" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
       <c r="C64" t="s">
         <v>69</v>
       </c>
@@ -8168,12 +8201,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>91</v>
+      </c>
       <c r="C65" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>91</v>
+      </c>
       <c r="B66" t="s">
         <v>71</v>
       </c>
@@ -8184,12 +8223,18 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>91</v>
+      </c>
       <c r="C67" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>91</v>
+      </c>
       <c r="C68" t="s">
         <v>74</v>
       </c>
@@ -8197,12 +8242,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>91</v>
+      </c>
       <c r="C69" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>91</v>
+      </c>
       <c r="C70" t="s">
         <v>76</v>
       </c>
@@ -8210,12 +8261,18 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>91</v>
+      </c>
       <c r="C71" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>91</v>
+      </c>
       <c r="C72" t="s">
         <v>78</v>
       </c>
@@ -8236,12 +8293,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8403,15 +8457,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE36113-C2DF-483C-81EB-AB3E1EF0A162}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F727651D-AE10-4FB1-A410-D3DAF16419A6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9d8d481b-b2d8-4ad2-9780-2aafe690507c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8435,17 +8500,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F727651D-AE10-4FB1-A410-D3DAF16419A6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE36113-C2DF-483C-81EB-AB3E1EF0A162}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9d8d481b-b2d8-4ad2-9780-2aafe690507c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>